<commit_message>
Greining notendahópa vol2 sælir
</commit_message>
<xml_diff>
--- a/Þarfagreiningaskýrsla/Lýsing Notendahóps/Greining notendahóps.xlsx
+++ b/Þarfagreiningaskýrsla/Lýsing Notendahóps/Greining notendahóps.xlsx
@@ -327,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,14 +394,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -500,7 +492,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -604,7 +596,7 @@
       <c r="E10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -615,7 +607,7 @@
       <c r="E11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -626,7 +618,7 @@
       <c r="E12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -637,7 +629,7 @@
       <c r="E13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -648,10 +640,12 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="12" t="n">
+        <v>10</v>
+      </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
@@ -660,13 +654,13 @@
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -677,7 +671,7 @@
       <c r="E17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -691,13 +685,13 @@
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="12" t="s">
         <v>30</v>
       </c>
@@ -706,7 +700,7 @@
       <c r="E20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="20" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="3" t="s">

</xml_diff>